<commit_message>
Typo corrections and formating
</commit_message>
<xml_diff>
--- a/Manual_Testing_Engeto_Pohlidalova.xlsx
+++ b/Manual_Testing_Engeto_Pohlidalova.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pohli\Desktop\ENGETO PYTHON\Manual-test-engeto-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7F6899-3AEE-486F-B019-214F77F65E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8C7346-86A4-4CE3-937A-19F1E9AB3DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23064" yWindow="0" windowWidth="24300" windowHeight="16656" activeTab="1" xr2:uid="{81C372EC-3577-45B6-BFE5-DD171F8BCF76}"/>
+    <workbookView xWindow="23760" yWindow="768" windowWidth="20436" windowHeight="13680" activeTab="1" xr2:uid="{81C372EC-3577-45B6-BFE5-DD171F8BCF76}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -825,7 +825,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -840,13 +840,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1261,7 +1254,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,10 +1987,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>